<commit_message>
Add content to HTML, CSS and JS files
</commit_message>
<xml_diff>
--- a/attendance-files/FA-II/FA-II (A) Attendance Sheet.xlsx
+++ b/attendance-files/FA-II/FA-II (A) Attendance Sheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="171">
   <si>
     <t>Indian Institute of Management Indore</t>
   </si>
@@ -90,6 +90,9 @@
     <t>Aditya Hartalkar</t>
   </si>
   <si>
+    <t xml:space="preserve">         A</t>
+  </si>
+  <si>
     <t>2024PGP033</t>
   </si>
   <si>
@@ -120,6 +123,9 @@
     <t xml:space="preserve">          A</t>
   </si>
   <si>
+    <t xml:space="preserve">        A</t>
+  </si>
+  <si>
     <t>2024PGP043</t>
   </si>
   <si>
@@ -192,9 +198,6 @@
     <t>C Dhayanand</t>
   </si>
   <si>
-    <t xml:space="preserve">         A</t>
-  </si>
-  <si>
     <t>2024PGP130</t>
   </si>
   <si>
@@ -219,6 +222,9 @@
     <t>Divyansh Anjan</t>
   </si>
   <si>
+    <t xml:space="preserve">           A</t>
+  </si>
+  <si>
     <t>2024PGP166</t>
   </si>
   <si>
@@ -231,6 +237,9 @@
     <t>Hardik Bhardwaj</t>
   </si>
   <si>
+    <t xml:space="preserve">            A</t>
+  </si>
+  <si>
     <t>2024PGP181</t>
   </si>
   <si>
@@ -259,6 +268,9 @@
   </si>
   <si>
     <t>K P Kishan Vaiyapuri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          </t>
   </si>
   <si>
     <t>2021IPM065</t>
@@ -887,7 +899,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -980,6 +992,9 @@
     </xf>
     <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -1688,7 +1703,7 @@
       </c>
       <c r="E9" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="33">
         <f t="shared" si="2"/>
@@ -1697,10 +1712,14 @@
       <c r="G9" s="34"/>
       <c r="H9" s="35"/>
       <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
+      <c r="J9" s="36" t="s">
+        <v>24</v>
+      </c>
       <c r="K9" s="35"/>
       <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
+      <c r="M9" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="N9" s="35"/>
       <c r="O9" s="35"/>
       <c r="P9" s="35"/>
@@ -1722,10 +1741,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10" s="25" t="s">
         <v>9</v>
@@ -1766,10 +1785,10 @@
         <v>5</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="25" t="s">
         <v>9</v>
@@ -1786,7 +1805,9 @@
       <c r="H11" s="35"/>
       <c r="I11" s="35"/>
       <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
+      <c r="K11" s="36" t="s">
+        <v>24</v>
+      </c>
       <c r="L11" s="35"/>
       <c r="M11" s="35"/>
       <c r="N11" s="35"/>
@@ -1810,31 +1831,35 @@
         <v>6</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D12" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F12" s="33">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G12" s="36" t="s">
-        <v>30</v>
+      <c r="G12" s="37" t="s">
+        <v>31</v>
       </c>
       <c r="H12" s="35"/>
       <c r="I12" s="35"/>
       <c r="J12" s="35"/>
       <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="35"/>
+      <c r="L12" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="N12" s="35"/>
       <c r="O12" s="35"/>
       <c r="P12" s="35"/>
@@ -1856,10 +1881,10 @@
         <v>7</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D13" s="25" t="s">
         <v>9</v>
@@ -1872,10 +1897,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G13" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="H13" s="35"/>
+      <c r="G13" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="36" t="s">
+        <v>35</v>
+      </c>
       <c r="I13" s="35"/>
       <c r="J13" s="35"/>
       <c r="K13" s="35"/>
@@ -1902,10 +1929,10 @@
         <v>8</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D14" s="25" t="s">
         <v>9</v>
@@ -1920,7 +1947,9 @@
       </c>
       <c r="G14" s="34"/>
       <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
+      <c r="I14" s="36" t="s">
+        <v>24</v>
+      </c>
       <c r="J14" s="35"/>
       <c r="K14" s="35"/>
       <c r="L14" s="35"/>
@@ -1946,17 +1975,17 @@
         <v>9</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D15" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F15" s="33">
         <f t="shared" si="2"/>
@@ -1967,8 +1996,12 @@
       <c r="I15" s="35"/>
       <c r="J15" s="35"/>
       <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
+      <c r="L15" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="M15" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="N15" s="35"/>
       <c r="O15" s="35"/>
       <c r="P15" s="35"/>
@@ -1990,10 +2023,10 @@
         <v>10</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D16" s="25" t="s">
         <v>9</v>
@@ -2034,17 +2067,17 @@
         <v>11</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D17" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="33">
         <f t="shared" si="2"/>
@@ -2055,7 +2088,9 @@
       <c r="I17" s="35"/>
       <c r="J17" s="35"/>
       <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
+      <c r="L17" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="M17" s="35"/>
       <c r="N17" s="35"/>
       <c r="O17" s="35"/>
@@ -2078,17 +2113,17 @@
         <v>12</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D18" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="33">
         <f t="shared" si="2"/>
@@ -2101,7 +2136,9 @@
       <c r="K18" s="35"/>
       <c r="L18" s="35"/>
       <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
+      <c r="N18" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="O18" s="35"/>
       <c r="P18" s="35"/>
       <c r="Q18" s="35"/>
@@ -2122,10 +2159,10 @@
         <v>13</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D19" s="25" t="s">
         <v>9</v>
@@ -2166,10 +2203,10 @@
         <v>14</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D20" s="25" t="s">
         <v>9</v>
@@ -2210,10 +2247,10 @@
         <v>15</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D21" s="25" t="s">
         <v>9</v>
@@ -2227,8 +2264,12 @@
         <v>0</v>
       </c>
       <c r="G21" s="34"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
+      <c r="H21" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" s="36" t="s">
+        <v>34</v>
+      </c>
       <c r="J21" s="35"/>
       <c r="K21" s="35"/>
       <c r="L21" s="35"/>
@@ -2254,10 +2295,10 @@
         <v>16</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D22" s="25" t="s">
         <v>9</v>
@@ -2298,10 +2339,10 @@
         <v>17</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D23" s="25" t="s">
         <v>9</v>
@@ -2316,7 +2357,9 @@
       </c>
       <c r="G23" s="34"/>
       <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
+      <c r="I23" s="36" t="s">
+        <v>34</v>
+      </c>
       <c r="J23" s="35"/>
       <c r="K23" s="35"/>
       <c r="L23" s="35"/>
@@ -2342,17 +2385,17 @@
         <v>18</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D24" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E24" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F24" s="33">
         <f t="shared" si="2"/>
@@ -2363,9 +2406,15 @@
       <c r="I24" s="35"/>
       <c r="J24" s="35"/>
       <c r="K24" s="35"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="35"/>
-      <c r="N24" s="35"/>
+      <c r="L24" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="M24" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="N24" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="O24" s="35"/>
       <c r="P24" s="35"/>
       <c r="Q24" s="35"/>
@@ -2386,10 +2435,10 @@
         <v>19</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C25" s="32" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D25" s="25" t="s">
         <v>9</v>
@@ -2402,13 +2451,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G25" s="36" t="s">
-        <v>58</v>
+      <c r="G25" s="37" t="s">
+        <v>24</v>
       </c>
       <c r="H25" s="35"/>
       <c r="I25" s="35"/>
       <c r="J25" s="35"/>
-      <c r="K25" s="35"/>
+      <c r="K25" s="36" t="s">
+        <v>34</v>
+      </c>
       <c r="L25" s="35"/>
       <c r="M25" s="35"/>
       <c r="N25" s="35"/>
@@ -2432,17 +2483,17 @@
         <v>20</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D26" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E26" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="33">
         <f t="shared" si="2"/>
@@ -2455,7 +2506,9 @@
       <c r="K26" s="35"/>
       <c r="L26" s="35"/>
       <c r="M26" s="35"/>
-      <c r="N26" s="35"/>
+      <c r="N26" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="O26" s="35"/>
       <c r="P26" s="35"/>
       <c r="Q26" s="35"/>
@@ -2476,17 +2529,17 @@
         <v>21</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C27" s="32" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D27" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E27" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F27" s="33">
         <f t="shared" si="2"/>
@@ -2497,8 +2550,12 @@
       <c r="I27" s="35"/>
       <c r="J27" s="35"/>
       <c r="K27" s="35"/>
-      <c r="L27" s="35"/>
-      <c r="M27" s="35"/>
+      <c r="L27" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="M27" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="N27" s="35"/>
       <c r="O27" s="35"/>
       <c r="P27" s="35"/>
@@ -2520,10 +2577,10 @@
         <v>22</v>
       </c>
       <c r="B28" s="31" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C28" s="32" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D28" s="25" t="s">
         <v>9</v>
@@ -2536,8 +2593,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G28" s="36" t="s">
-        <v>33</v>
+      <c r="G28" s="37" t="s">
+        <v>34</v>
       </c>
       <c r="H28" s="35"/>
       <c r="I28" s="35"/>
@@ -2566,17 +2623,17 @@
         <v>23</v>
       </c>
       <c r="B29" s="31" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C29" s="32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D29" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E29" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" s="33">
         <f t="shared" si="2"/>
@@ -2584,12 +2641,16 @@
       </c>
       <c r="G29" s="34"/>
       <c r="H29" s="35"/>
-      <c r="I29" s="35"/>
+      <c r="I29" s="36" t="s">
+        <v>68</v>
+      </c>
       <c r="J29" s="35"/>
       <c r="K29" s="35"/>
       <c r="L29" s="35"/>
       <c r="M29" s="35"/>
-      <c r="N29" s="35"/>
+      <c r="N29" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="O29" s="35"/>
       <c r="P29" s="35"/>
       <c r="Q29" s="35"/>
@@ -2610,30 +2671,38 @@
         <v>24</v>
       </c>
       <c r="B30" s="31" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C30" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F30" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G30" s="34"/>
+      <c r="H30" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="I30" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="D30" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F30" s="33">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G30" s="34"/>
-      <c r="H30" s="35"/>
-      <c r="I30" s="35"/>
-      <c r="J30" s="35"/>
+      <c r="J30" s="36" t="s">
+        <v>24</v>
+      </c>
       <c r="K30" s="35"/>
       <c r="L30" s="35"/>
       <c r="M30" s="35"/>
-      <c r="N30" s="35"/>
+      <c r="N30" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="O30" s="35"/>
       <c r="P30" s="35"/>
       <c r="Q30" s="35"/>
@@ -2654,10 +2723,10 @@
         <v>25</v>
       </c>
       <c r="B31" s="31" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C31" s="32" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D31" s="25" t="s">
         <v>9</v>
@@ -2672,9 +2741,15 @@
       </c>
       <c r="G31" s="34"/>
       <c r="H31" s="35"/>
-      <c r="I31" s="35"/>
-      <c r="J31" s="35"/>
-      <c r="K31" s="35"/>
+      <c r="I31" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="J31" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="K31" s="36" t="s">
+        <v>34</v>
+      </c>
       <c r="L31" s="35"/>
       <c r="M31" s="35"/>
       <c r="N31" s="35"/>
@@ -2698,17 +2773,17 @@
         <v>26</v>
       </c>
       <c r="B32" s="31" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C32" s="32" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D32" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E32" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" s="33">
         <f t="shared" si="2"/>
@@ -2717,9 +2792,13 @@
       <c r="G32" s="34"/>
       <c r="H32" s="35"/>
       <c r="I32" s="35"/>
-      <c r="J32" s="35"/>
+      <c r="J32" s="36" t="s">
+        <v>34</v>
+      </c>
       <c r="K32" s="35"/>
-      <c r="L32" s="35"/>
+      <c r="L32" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="M32" s="35"/>
       <c r="N32" s="35"/>
       <c r="O32" s="35"/>
@@ -2742,10 +2821,10 @@
         <v>27</v>
       </c>
       <c r="B33" s="31" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C33" s="32" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D33" s="25" t="s">
         <v>9</v>
@@ -2786,17 +2865,17 @@
         <v>28</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D34" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E34" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34" s="33">
         <f t="shared" si="2"/>
@@ -2807,7 +2886,9 @@
       <c r="I34" s="35"/>
       <c r="J34" s="35"/>
       <c r="K34" s="35"/>
-      <c r="L34" s="35"/>
+      <c r="L34" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="M34" s="35"/>
       <c r="N34" s="35"/>
       <c r="O34" s="35"/>
@@ -2830,10 +2911,10 @@
         <v>29</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C35" s="32" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D35" s="25" t="s">
         <v>9</v>
@@ -2847,10 +2928,18 @@
         <v>0</v>
       </c>
       <c r="G35" s="34"/>
-      <c r="H35" s="35"/>
-      <c r="I35" s="35"/>
-      <c r="J35" s="35"/>
-      <c r="K35" s="35"/>
+      <c r="H35" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="I35" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K35" s="36" t="s">
+        <v>34</v>
+      </c>
       <c r="L35" s="35"/>
       <c r="M35" s="35"/>
       <c r="N35" s="35"/>
@@ -2874,10 +2963,10 @@
         <v>30</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C36" s="32" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D36" s="25" t="s">
         <v>9</v>
@@ -2893,7 +2982,9 @@
       <c r="G36" s="34"/>
       <c r="H36" s="35"/>
       <c r="I36" s="35"/>
-      <c r="J36" s="35"/>
+      <c r="J36" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="K36" s="35"/>
       <c r="L36" s="35"/>
       <c r="M36" s="35"/>
@@ -2918,10 +3009,10 @@
         <v>31</v>
       </c>
       <c r="B37" s="31" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D37" s="25" t="s">
         <v>9</v>
@@ -2935,10 +3026,18 @@
         <v>0</v>
       </c>
       <c r="G37" s="34"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="35"/>
-      <c r="K37" s="35"/>
+      <c r="H37" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="I37" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="J37" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K37" s="36" t="s">
+        <v>68</v>
+      </c>
       <c r="L37" s="35"/>
       <c r="M37" s="35"/>
       <c r="N37" s="35"/>
@@ -2962,17 +3061,17 @@
         <v>32</v>
       </c>
       <c r="B38" s="31" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C38" s="32" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D38" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E38" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" s="33">
         <f t="shared" si="2"/>
@@ -2981,11 +3080,15 @@
       <c r="G38" s="34"/>
       <c r="H38" s="35"/>
       <c r="I38" s="35"/>
-      <c r="J38" s="35"/>
+      <c r="J38" s="36" t="s">
+        <v>68</v>
+      </c>
       <c r="K38" s="35"/>
       <c r="L38" s="35"/>
       <c r="M38" s="35"/>
-      <c r="N38" s="35"/>
+      <c r="N38" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="O38" s="35"/>
       <c r="P38" s="35"/>
       <c r="Q38" s="35"/>
@@ -3006,10 +3109,10 @@
         <v>33</v>
       </c>
       <c r="B39" s="31" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C39" s="32" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D39" s="25" t="s">
         <v>9</v>
@@ -3050,10 +3153,10 @@
         <v>34</v>
       </c>
       <c r="B40" s="31" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D40" s="25" t="s">
         <v>9</v>
@@ -3094,10 +3197,10 @@
         <v>35</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C41" s="32" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D41" s="25" t="s">
         <v>9</v>
@@ -3111,7 +3214,9 @@
         <v>0</v>
       </c>
       <c r="G41" s="34"/>
-      <c r="H41" s="35"/>
+      <c r="H41" s="36" t="s">
+        <v>24</v>
+      </c>
       <c r="I41" s="35"/>
       <c r="J41" s="35"/>
       <c r="K41" s="35"/>
@@ -3138,17 +3243,17 @@
         <v>36</v>
       </c>
       <c r="B42" s="31" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C42" s="32" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D42" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E42" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42" s="33">
         <f t="shared" si="2"/>
@@ -3161,7 +3266,9 @@
       <c r="K42" s="35"/>
       <c r="L42" s="35"/>
       <c r="M42" s="35"/>
-      <c r="N42" s="35"/>
+      <c r="N42" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="O42" s="35"/>
       <c r="P42" s="35"/>
       <c r="Q42" s="35"/>
@@ -3182,10 +3289,10 @@
         <v>37</v>
       </c>
       <c r="B43" s="31" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D43" s="25" t="s">
         <v>9</v>
@@ -3226,29 +3333,35 @@
         <v>38</v>
       </c>
       <c r="B44" s="31" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C44" s="32" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D44" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E44" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F44" s="33">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G44" s="34"/>
-      <c r="H44" s="35"/>
+      <c r="H44" s="36" t="s">
+        <v>24</v>
+      </c>
       <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="J44" s="36" t="s">
+        <v>68</v>
+      </c>
       <c r="K44" s="35"/>
       <c r="L44" s="35"/>
-      <c r="M44" s="35"/>
+      <c r="M44" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="N44" s="35"/>
       <c r="O44" s="35"/>
       <c r="P44" s="35"/>
@@ -3270,17 +3383,17 @@
         <v>39</v>
       </c>
       <c r="B45" s="31" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C45" s="32" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D45" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E45" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45" s="33">
         <f t="shared" si="2"/>
@@ -3292,7 +3405,9 @@
       <c r="J45" s="35"/>
       <c r="K45" s="35"/>
       <c r="L45" s="35"/>
-      <c r="M45" s="35"/>
+      <c r="M45" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="N45" s="35"/>
       <c r="O45" s="35"/>
       <c r="P45" s="35"/>
@@ -3314,17 +3429,17 @@
         <v>40</v>
       </c>
       <c r="B46" s="31" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C46" s="32" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D46" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E46" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46" s="33">
         <f t="shared" si="2"/>
@@ -3335,7 +3450,9 @@
       <c r="I46" s="35"/>
       <c r="J46" s="35"/>
       <c r="K46" s="35"/>
-      <c r="L46" s="35"/>
+      <c r="L46" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="M46" s="35"/>
       <c r="N46" s="35"/>
       <c r="O46" s="35"/>
@@ -3358,10 +3475,10 @@
         <v>41</v>
       </c>
       <c r="B47" s="31" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C47" s="32" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D47" s="25" t="s">
         <v>9</v>
@@ -3402,10 +3519,10 @@
         <v>42</v>
       </c>
       <c r="B48" s="31" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C48" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D48" s="25" t="s">
         <v>9</v>
@@ -3446,17 +3563,17 @@
         <v>43</v>
       </c>
       <c r="B49" s="31" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C49" s="32" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D49" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E49" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F49" s="33">
         <f t="shared" si="2"/>
@@ -3464,10 +3581,14 @@
       </c>
       <c r="G49" s="34"/>
       <c r="H49" s="35"/>
-      <c r="I49" s="35"/>
+      <c r="I49" s="36" t="s">
+        <v>68</v>
+      </c>
       <c r="J49" s="35"/>
       <c r="K49" s="35"/>
-      <c r="L49" s="35"/>
+      <c r="L49" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="M49" s="35"/>
       <c r="N49" s="35"/>
       <c r="O49" s="35"/>
@@ -3490,17 +3611,17 @@
         <v>44</v>
       </c>
       <c r="B50" s="31" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D50" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E50" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50" s="33">
         <f t="shared" si="2"/>
@@ -3511,7 +3632,9 @@
       <c r="I50" s="35"/>
       <c r="J50" s="35"/>
       <c r="K50" s="35"/>
-      <c r="L50" s="35"/>
+      <c r="L50" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="M50" s="35"/>
       <c r="N50" s="35"/>
       <c r="O50" s="35"/>
@@ -3534,10 +3657,10 @@
         <v>45</v>
       </c>
       <c r="B51" s="31" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C51" s="32" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D51" s="25" t="s">
         <v>9</v>
@@ -3578,29 +3701,33 @@
         <v>46</v>
       </c>
       <c r="B52" s="31" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C52" s="32" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D52" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E52" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F52" s="33">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G52" s="34"/>
-      <c r="H52" s="35"/>
+      <c r="H52" s="36" t="s">
+        <v>24</v>
+      </c>
       <c r="I52" s="35"/>
       <c r="J52" s="35"/>
       <c r="K52" s="35"/>
       <c r="L52" s="35"/>
-      <c r="M52" s="35"/>
+      <c r="M52" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="N52" s="35"/>
       <c r="O52" s="35"/>
       <c r="P52" s="35"/>
@@ -3622,10 +3749,10 @@
         <v>47</v>
       </c>
       <c r="B53" s="31" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C53" s="32" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D53" s="25" t="s">
         <v>9</v>
@@ -3666,17 +3793,17 @@
         <v>48</v>
       </c>
       <c r="B54" s="31" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C54" s="32" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D54" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E54" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F54" s="33">
         <f t="shared" si="2"/>
@@ -3684,10 +3811,14 @@
       </c>
       <c r="G54" s="34"/>
       <c r="H54" s="35"/>
-      <c r="I54" s="35"/>
+      <c r="I54" s="36" t="s">
+        <v>68</v>
+      </c>
       <c r="J54" s="35"/>
       <c r="K54" s="35"/>
-      <c r="L54" s="35"/>
+      <c r="L54" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="M54" s="35"/>
       <c r="N54" s="35"/>
       <c r="O54" s="35"/>
@@ -3710,17 +3841,17 @@
         <v>49</v>
       </c>
       <c r="B55" s="31" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C55" s="32" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D55" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E55" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F55" s="33">
         <f t="shared" si="2"/>
@@ -3729,9 +3860,13 @@
       <c r="G55" s="34"/>
       <c r="H55" s="35"/>
       <c r="I55" s="35"/>
-      <c r="J55" s="35"/>
+      <c r="J55" s="36" t="s">
+        <v>34</v>
+      </c>
       <c r="K55" s="35"/>
-      <c r="L55" s="35"/>
+      <c r="L55" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="M55" s="35"/>
       <c r="N55" s="35"/>
       <c r="O55" s="35"/>
@@ -3754,17 +3889,17 @@
         <v>50</v>
       </c>
       <c r="B56" s="31" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C56" s="32" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D56" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E56" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F56" s="33">
         <f t="shared" si="2"/>
@@ -3777,7 +3912,9 @@
       <c r="K56" s="35"/>
       <c r="L56" s="35"/>
       <c r="M56" s="35"/>
-      <c r="N56" s="35"/>
+      <c r="N56" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="O56" s="35"/>
       <c r="P56" s="35"/>
       <c r="Q56" s="35"/>
@@ -3798,10 +3935,10 @@
         <v>51</v>
       </c>
       <c r="B57" s="31" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C57" s="32" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D57" s="25" t="s">
         <v>9</v>
@@ -3816,7 +3953,9 @@
       </c>
       <c r="G57" s="34"/>
       <c r="H57" s="35"/>
-      <c r="I57" s="35"/>
+      <c r="I57" s="36" t="s">
+        <v>68</v>
+      </c>
       <c r="J57" s="35"/>
       <c r="K57" s="35"/>
       <c r="L57" s="35"/>
@@ -3842,10 +3981,10 @@
         <v>52</v>
       </c>
       <c r="B58" s="31" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C58" s="32" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D58" s="25" t="s">
         <v>9</v>
@@ -3859,7 +3998,9 @@
         <v>0</v>
       </c>
       <c r="G58" s="34"/>
-      <c r="H58" s="35"/>
+      <c r="H58" s="36" t="s">
+        <v>34</v>
+      </c>
       <c r="I58" s="35"/>
       <c r="J58" s="35"/>
       <c r="K58" s="35"/>
@@ -3886,10 +4027,10 @@
         <v>53</v>
       </c>
       <c r="B59" s="31" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C59" s="32" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D59" s="25" t="s">
         <v>9</v>
@@ -3930,10 +4071,10 @@
         <v>54</v>
       </c>
       <c r="B60" s="31" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C60" s="32" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D60" s="25" t="s">
         <v>9</v>
@@ -3974,29 +4115,35 @@
         <v>55</v>
       </c>
       <c r="B61" s="31" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C61" s="32" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D61" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E61" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F61" s="33">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G61" s="34"/>
-      <c r="H61" s="35"/>
+      <c r="H61" s="36" t="s">
+        <v>68</v>
+      </c>
       <c r="I61" s="35"/>
       <c r="J61" s="35"/>
       <c r="K61" s="35"/>
-      <c r="L61" s="35"/>
-      <c r="M61" s="35"/>
+      <c r="L61" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="M61" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="N61" s="35"/>
       <c r="O61" s="35"/>
       <c r="P61" s="35"/>
@@ -4018,17 +4165,17 @@
         <v>56</v>
       </c>
       <c r="B62" s="31" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C62" s="32" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D62" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E62" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F62" s="33">
         <f t="shared" si="2"/>
@@ -4039,8 +4186,12 @@
       <c r="I62" s="35"/>
       <c r="J62" s="35"/>
       <c r="K62" s="35"/>
-      <c r="L62" s="35"/>
-      <c r="M62" s="35"/>
+      <c r="L62" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="M62" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="N62" s="35"/>
       <c r="O62" s="35"/>
       <c r="P62" s="35"/>
@@ -4062,29 +4213,33 @@
         <v>57</v>
       </c>
       <c r="B63" s="31" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C63" s="32" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D63" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E63" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F63" s="33">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G63" s="34"/>
-      <c r="H63" s="35"/>
+      <c r="H63" s="36" t="s">
+        <v>68</v>
+      </c>
       <c r="I63" s="35"/>
       <c r="J63" s="35"/>
       <c r="K63" s="35"/>
       <c r="L63" s="35"/>
-      <c r="M63" s="35"/>
+      <c r="M63" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="N63" s="35"/>
       <c r="O63" s="35"/>
       <c r="P63" s="35"/>
@@ -4106,17 +4261,17 @@
         <v>58</v>
       </c>
       <c r="B64" s="31" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C64" s="32" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D64" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E64" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F64" s="33">
         <f t="shared" si="2"/>
@@ -4127,7 +4282,9 @@
       <c r="I64" s="35"/>
       <c r="J64" s="35"/>
       <c r="K64" s="35"/>
-      <c r="L64" s="35"/>
+      <c r="L64" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="M64" s="35"/>
       <c r="N64" s="35"/>
       <c r="O64" s="35"/>
@@ -4150,10 +4307,10 @@
         <v>59</v>
       </c>
       <c r="B65" s="31" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C65" s="32" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D65" s="25" t="s">
         <v>9</v>
@@ -4166,8 +4323,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G65" s="36" t="s">
-        <v>58</v>
+      <c r="G65" s="37" t="s">
+        <v>24</v>
       </c>
       <c r="H65" s="35"/>
       <c r="I65" s="35"/>
@@ -4196,17 +4353,17 @@
         <v>60</v>
       </c>
       <c r="B66" s="31" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C66" s="32" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D66" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E66" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F66" s="33">
         <f t="shared" si="2"/>
@@ -4217,7 +4374,9 @@
       <c r="I66" s="35"/>
       <c r="J66" s="35"/>
       <c r="K66" s="35"/>
-      <c r="L66" s="35"/>
+      <c r="L66" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="M66" s="35"/>
       <c r="N66" s="35"/>
       <c r="O66" s="35"/>
@@ -4240,28 +4399,32 @@
         <v>61</v>
       </c>
       <c r="B67" s="31" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C67" s="32" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D67" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E67" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F67" s="33">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G67" s="34"/>
-      <c r="H67" s="35"/>
+      <c r="H67" s="36" t="s">
+        <v>34</v>
+      </c>
       <c r="I67" s="35"/>
       <c r="J67" s="35"/>
       <c r="K67" s="35"/>
-      <c r="L67" s="35"/>
+      <c r="L67" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="M67" s="35"/>
       <c r="N67" s="35"/>
       <c r="O67" s="35"/>
@@ -4284,17 +4447,17 @@
         <v>62</v>
       </c>
       <c r="B68" s="31" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C68" s="32" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D68" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E68" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F68" s="33">
         <f t="shared" si="2"/>
@@ -4307,7 +4470,9 @@
       <c r="K68" s="35"/>
       <c r="L68" s="35"/>
       <c r="M68" s="35"/>
-      <c r="N68" s="35"/>
+      <c r="N68" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="O68" s="35"/>
       <c r="P68" s="35"/>
       <c r="Q68" s="35"/>
@@ -4328,17 +4493,17 @@
         <v>63</v>
       </c>
       <c r="B69" s="31" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C69" s="32" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D69" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E69" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F69" s="33">
         <f t="shared" si="2"/>
@@ -4349,7 +4514,9 @@
       <c r="I69" s="35"/>
       <c r="J69" s="35"/>
       <c r="K69" s="35"/>
-      <c r="L69" s="35"/>
+      <c r="L69" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="M69" s="35"/>
       <c r="N69" s="35"/>
       <c r="O69" s="35"/>
@@ -4372,17 +4539,17 @@
         <v>64</v>
       </c>
       <c r="B70" s="31" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C70" s="32" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D70" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E70" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F70" s="33">
         <f t="shared" si="2"/>
@@ -4393,7 +4560,9 @@
       <c r="I70" s="35"/>
       <c r="J70" s="35"/>
       <c r="K70" s="35"/>
-      <c r="L70" s="35"/>
+      <c r="L70" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="M70" s="35"/>
       <c r="N70" s="35"/>
       <c r="O70" s="35"/>
@@ -4416,17 +4585,17 @@
         <v>65</v>
       </c>
       <c r="B71" s="31" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C71" s="32" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D71" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E71" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F71" s="33">
         <f t="shared" si="2"/>
@@ -4438,7 +4607,9 @@
       <c r="J71" s="35"/>
       <c r="K71" s="35"/>
       <c r="L71" s="35"/>
-      <c r="M71" s="35"/>
+      <c r="M71" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="N71" s="35"/>
       <c r="O71" s="35"/>
       <c r="P71" s="35"/>
@@ -4460,17 +4631,17 @@
         <v>66</v>
       </c>
       <c r="B72" s="31" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C72" s="32" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D72" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E72" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F72" s="33">
         <f t="shared" si="2"/>
@@ -4479,9 +4650,13 @@
       <c r="G72" s="34"/>
       <c r="H72" s="35"/>
       <c r="I72" s="35"/>
-      <c r="J72" s="35"/>
+      <c r="J72" s="36" t="s">
+        <v>24</v>
+      </c>
       <c r="K72" s="35"/>
-      <c r="L72" s="35"/>
+      <c r="L72" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="M72" s="35"/>
       <c r="N72" s="35"/>
       <c r="O72" s="35"/>
@@ -4504,10 +4679,10 @@
         <v>67</v>
       </c>
       <c r="B73" s="31" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C73" s="32" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D73" s="25" t="s">
         <v>9</v>
@@ -4522,7 +4697,9 @@
       </c>
       <c r="G73" s="34"/>
       <c r="H73" s="35"/>
-      <c r="I73" s="35"/>
+      <c r="I73" s="36" t="s">
+        <v>34</v>
+      </c>
       <c r="J73" s="35"/>
       <c r="K73" s="35"/>
       <c r="L73" s="35"/>
@@ -4548,10 +4725,10 @@
         <v>68</v>
       </c>
       <c r="B74" s="31" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C74" s="32" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="D74" s="25" t="s">
         <v>9</v>
@@ -4566,8 +4743,12 @@
       </c>
       <c r="G74" s="34"/>
       <c r="H74" s="35"/>
-      <c r="I74" s="35"/>
-      <c r="J74" s="35"/>
+      <c r="I74" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="J74" s="36" t="s">
+        <v>34</v>
+      </c>
       <c r="K74" s="35"/>
       <c r="L74" s="35"/>
       <c r="M74" s="35"/>
@@ -4592,28 +4773,36 @@
         <v>69</v>
       </c>
       <c r="B75" s="31" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C75" s="32" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="D75" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E75" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F75" s="33">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G75" s="34"/>
-      <c r="H75" s="35"/>
-      <c r="I75" s="35"/>
+      <c r="H75" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="I75" s="36" t="s">
+        <v>34</v>
+      </c>
       <c r="J75" s="35"/>
-      <c r="K75" s="35"/>
-      <c r="L75" s="35"/>
+      <c r="K75" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="L75" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="M75" s="35"/>
       <c r="N75" s="35"/>
       <c r="O75" s="35"/>
@@ -4636,17 +4825,17 @@
         <v>70</v>
       </c>
       <c r="B76" s="31" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C76" s="32" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="D76" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E76" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F76" s="33">
         <f t="shared" si="2"/>
@@ -4656,9 +4845,13 @@
       <c r="H76" s="35"/>
       <c r="I76" s="35"/>
       <c r="J76" s="35"/>
-      <c r="K76" s="35"/>
+      <c r="K76" s="36" t="s">
+        <v>34</v>
+      </c>
       <c r="L76" s="35"/>
-      <c r="M76" s="35"/>
+      <c r="M76" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="N76" s="35"/>
       <c r="O76" s="35"/>
       <c r="P76" s="35"/>
@@ -4680,10 +4873,10 @@
         <v>71</v>
       </c>
       <c r="B77" s="31" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C77" s="32" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="D77" s="25" t="s">
         <v>9</v>
@@ -4700,7 +4893,9 @@
       <c r="H77" s="35"/>
       <c r="I77" s="35"/>
       <c r="J77" s="35"/>
-      <c r="K77" s="35"/>
+      <c r="K77" s="36" t="s">
+        <v>68</v>
+      </c>
       <c r="L77" s="35"/>
       <c r="M77" s="35"/>
       <c r="N77" s="35"/>
@@ -4724,10 +4919,10 @@
         <v>72</v>
       </c>
       <c r="B78" s="31" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C78" s="32" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="D78" s="25" t="s">
         <v>9</v>
@@ -4768,17 +4963,17 @@
         <v>73</v>
       </c>
       <c r="B79" s="31" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C79" s="32" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="D79" s="25" t="s">
         <v>9</v>
       </c>
       <c r="E79" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F79" s="33">
         <f t="shared" si="2"/>
@@ -4790,7 +4985,9 @@
       <c r="J79" s="35"/>
       <c r="K79" s="35"/>
       <c r="L79" s="35"/>
-      <c r="M79" s="35"/>
+      <c r="M79" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="N79" s="35"/>
       <c r="O79" s="35"/>
       <c r="P79" s="35"/>
@@ -5001,8 +5198,8 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="B85" s="37"/>
-      <c r="C85" s="37"/>
+      <c r="B85" s="38"/>
+      <c r="C85" s="38"/>
       <c r="D85" s="26"/>
       <c r="E85" s="26" t="str">
         <f t="shared" si="1"/>
@@ -5039,8 +5236,8 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="B86" s="37"/>
-      <c r="C86" s="37"/>
+      <c r="B86" s="38"/>
+      <c r="C86" s="38"/>
       <c r="D86" s="26"/>
       <c r="E86" s="26" t="str">
         <f t="shared" si="1"/>
@@ -5077,8 +5274,8 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="B87" s="37"/>
-      <c r="C87" s="37"/>
+      <c r="B87" s="38"/>
+      <c r="C87" s="38"/>
       <c r="D87" s="26"/>
       <c r="E87" s="26" t="str">
         <f t="shared" si="1"/>
@@ -5115,8 +5312,8 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="B88" s="37"/>
-      <c r="C88" s="37"/>
+      <c r="B88" s="38"/>
+      <c r="C88" s="38"/>
       <c r="D88" s="26"/>
       <c r="E88" s="26" t="str">
         <f t="shared" si="1"/>
@@ -5153,8 +5350,8 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="B89" s="37"/>
-      <c r="C89" s="37"/>
+      <c r="B89" s="38"/>
+      <c r="C89" s="38"/>
       <c r="D89" s="26"/>
       <c r="E89" s="26" t="str">
         <f t="shared" si="1"/>
@@ -5191,8 +5388,8 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="B90" s="37"/>
-      <c r="C90" s="37"/>
+      <c r="B90" s="38"/>
+      <c r="C90" s="38"/>
       <c r="D90" s="26"/>
       <c r="E90" s="26" t="str">
         <f t="shared" si="1"/>
@@ -5229,8 +5426,8 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="B91" s="37"/>
-      <c r="C91" s="37"/>
+      <c r="B91" s="38"/>
+      <c r="C91" s="38"/>
       <c r="D91" s="26"/>
       <c r="E91" s="26" t="str">
         <f t="shared" si="1"/>
@@ -5267,8 +5464,8 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="B92" s="37"/>
-      <c r="C92" s="37"/>
+      <c r="B92" s="38"/>
+      <c r="C92" s="38"/>
       <c r="D92" s="26"/>
       <c r="E92" s="26" t="str">
         <f t="shared" si="1"/>
@@ -5305,8 +5502,8 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="B93" s="37"/>
-      <c r="C93" s="37"/>
+      <c r="B93" s="38"/>
+      <c r="C93" s="38"/>
       <c r="D93" s="26"/>
       <c r="E93" s="26" t="str">
         <f t="shared" si="1"/>
@@ -5343,8 +5540,8 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="B94" s="37"/>
-      <c r="C94" s="37"/>
+      <c r="B94" s="38"/>
+      <c r="C94" s="38"/>
       <c r="D94" s="26"/>
       <c r="E94" s="26" t="str">
         <f t="shared" si="1"/>
@@ -5381,8 +5578,8 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="B95" s="37"/>
-      <c r="C95" s="37"/>
+      <c r="B95" s="38"/>
+      <c r="C95" s="38"/>
       <c r="D95" s="26"/>
       <c r="E95" s="26" t="str">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Updating attendance files 9th feb
</commit_message>
<xml_diff>
--- a/attendance-files/FA-II/FA-II (A) Attendance Sheet.xlsx
+++ b/attendance-files/FA-II/FA-II (A) Attendance Sheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="171">
   <si>
     <t>Indian Institute of Management Indore</t>
   </si>
@@ -1841,7 +1841,7 @@
       </c>
       <c r="E12" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F12" s="33">
         <f t="shared" si="2"/>
@@ -1862,7 +1862,9 @@
       </c>
       <c r="N12" s="35"/>
       <c r="O12" s="35"/>
-      <c r="P12" s="35"/>
+      <c r="P12" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="Q12" s="35"/>
       <c r="R12" s="35"/>
       <c r="S12" s="35"/>
@@ -1891,7 +1893,7 @@
       </c>
       <c r="E13" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="33">
         <f t="shared" si="2"/>
@@ -1910,7 +1912,9 @@
       <c r="M13" s="35"/>
       <c r="N13" s="35"/>
       <c r="O13" s="35"/>
-      <c r="P13" s="35"/>
+      <c r="P13" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="Q13" s="35"/>
       <c r="R13" s="35"/>
       <c r="S13" s="35"/>
@@ -2077,7 +2081,7 @@
       </c>
       <c r="E17" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" s="33">
         <f t="shared" si="2"/>
@@ -2093,7 +2097,9 @@
       </c>
       <c r="M17" s="35"/>
       <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
+      <c r="O17" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="P17" s="35"/>
       <c r="Q17" s="35"/>
       <c r="R17" s="35"/>
@@ -2257,7 +2263,7 @@
       </c>
       <c r="E21" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="33">
         <f t="shared" si="2"/>
@@ -2275,7 +2281,9 @@
       <c r="L21" s="35"/>
       <c r="M21" s="35"/>
       <c r="N21" s="35"/>
-      <c r="O21" s="35"/>
+      <c r="O21" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="P21" s="35"/>
       <c r="Q21" s="35"/>
       <c r="R21" s="35"/>
@@ -2395,7 +2403,7 @@
       </c>
       <c r="E24" s="26">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F24" s="33">
         <f t="shared" si="2"/>
@@ -2415,7 +2423,9 @@
       <c r="N24" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="O24" s="35"/>
+      <c r="O24" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="P24" s="35"/>
       <c r="Q24" s="35"/>
       <c r="R24" s="35"/>
@@ -2493,7 +2503,7 @@
       </c>
       <c r="E26" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F26" s="33">
         <f t="shared" si="2"/>
@@ -2509,7 +2519,9 @@
       <c r="N26" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="O26" s="35"/>
+      <c r="O26" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="P26" s="35"/>
       <c r="Q26" s="35"/>
       <c r="R26" s="35"/>
@@ -2831,7 +2843,7 @@
       </c>
       <c r="E33" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" s="33">
         <f t="shared" si="2"/>
@@ -2845,7 +2857,9 @@
       <c r="L33" s="35"/>
       <c r="M33" s="35"/>
       <c r="N33" s="35"/>
-      <c r="O33" s="35"/>
+      <c r="O33" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="P33" s="35"/>
       <c r="Q33" s="35"/>
       <c r="R33" s="35"/>
@@ -2875,7 +2889,7 @@
       </c>
       <c r="E34" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F34" s="33">
         <f t="shared" si="2"/>
@@ -2891,8 +2905,12 @@
       </c>
       <c r="M34" s="35"/>
       <c r="N34" s="35"/>
-      <c r="O34" s="35"/>
-      <c r="P34" s="35"/>
+      <c r="O34" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="P34" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="Q34" s="35"/>
       <c r="R34" s="35"/>
       <c r="S34" s="35"/>
@@ -3119,7 +3137,7 @@
       </c>
       <c r="E39" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" s="33">
         <f t="shared" si="2"/>
@@ -3134,7 +3152,9 @@
       <c r="M39" s="35"/>
       <c r="N39" s="35"/>
       <c r="O39" s="35"/>
-      <c r="P39" s="35"/>
+      <c r="P39" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="Q39" s="35"/>
       <c r="R39" s="35"/>
       <c r="S39" s="35"/>
@@ -3343,7 +3363,7 @@
       </c>
       <c r="E44" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F44" s="33">
         <f t="shared" si="2"/>
@@ -3364,7 +3384,9 @@
       </c>
       <c r="N44" s="35"/>
       <c r="O44" s="35"/>
-      <c r="P44" s="35"/>
+      <c r="P44" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="Q44" s="35"/>
       <c r="R44" s="35"/>
       <c r="S44" s="35"/>
@@ -3621,7 +3643,7 @@
       </c>
       <c r="E50" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F50" s="33">
         <f t="shared" si="2"/>
@@ -3638,7 +3660,9 @@
       <c r="M50" s="35"/>
       <c r="N50" s="35"/>
       <c r="O50" s="35"/>
-      <c r="P50" s="35"/>
+      <c r="P50" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="Q50" s="35"/>
       <c r="R50" s="35"/>
       <c r="S50" s="35"/>
@@ -3803,7 +3827,7 @@
       </c>
       <c r="E54" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F54" s="33">
         <f t="shared" si="2"/>
@@ -3822,7 +3846,9 @@
       <c r="M54" s="35"/>
       <c r="N54" s="35"/>
       <c r="O54" s="35"/>
-      <c r="P54" s="35"/>
+      <c r="P54" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="Q54" s="35"/>
       <c r="R54" s="35"/>
       <c r="S54" s="35"/>
@@ -4125,7 +4151,7 @@
       </c>
       <c r="E61" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F61" s="33">
         <f t="shared" si="2"/>
@@ -4145,7 +4171,9 @@
         <v>9</v>
       </c>
       <c r="N61" s="35"/>
-      <c r="O61" s="35"/>
+      <c r="O61" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="P61" s="35"/>
       <c r="Q61" s="35"/>
       <c r="R61" s="35"/>
@@ -4223,7 +4251,7 @@
       </c>
       <c r="E63" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F63" s="33">
         <f t="shared" si="2"/>
@@ -4241,7 +4269,9 @@
         <v>9</v>
       </c>
       <c r="N63" s="35"/>
-      <c r="O63" s="35"/>
+      <c r="O63" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="P63" s="35"/>
       <c r="Q63" s="35"/>
       <c r="R63" s="35"/>
@@ -4457,7 +4487,7 @@
       </c>
       <c r="E68" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F68" s="33">
         <f t="shared" si="2"/>
@@ -4473,8 +4503,12 @@
       <c r="N68" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="O68" s="35"/>
-      <c r="P68" s="35"/>
+      <c r="O68" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="P68" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="Q68" s="35"/>
       <c r="R68" s="35"/>
       <c r="S68" s="35"/>

</xml_diff>

<commit_message>
Updating attendance files 19th feb
</commit_message>
<xml_diff>
--- a/attendance-files/FA-II/FA-II (A) Attendance Sheet.xlsx
+++ b/attendance-files/FA-II/FA-II (A) Attendance Sheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="171">
   <si>
     <t>Indian Institute of Management Indore</t>
   </si>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="E8" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8" s="33">
         <f t="shared" si="2"/>
@@ -1675,8 +1675,12 @@
       <c r="N8" s="35"/>
       <c r="O8" s="35"/>
       <c r="P8" s="35"/>
-      <c r="Q8" s="35"/>
-      <c r="R8" s="35"/>
+      <c r="Q8" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="R8" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="S8" s="35"/>
       <c r="T8" s="35"/>
       <c r="U8" s="35"/>
@@ -1841,7 +1845,7 @@
       </c>
       <c r="E12" s="26">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F12" s="33">
         <f t="shared" si="2"/>
@@ -1867,7 +1871,9 @@
       </c>
       <c r="Q12" s="35"/>
       <c r="R12" s="35"/>
-      <c r="S12" s="35"/>
+      <c r="S12" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="T12" s="35"/>
       <c r="U12" s="35"/>
       <c r="V12" s="35"/>
@@ -2129,7 +2135,7 @@
       </c>
       <c r="E18" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F18" s="33">
         <f t="shared" si="2"/>
@@ -2147,7 +2153,9 @@
       </c>
       <c r="O18" s="35"/>
       <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
+      <c r="Q18" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="R18" s="35"/>
       <c r="S18" s="35"/>
       <c r="T18" s="35"/>
@@ -2263,7 +2271,7 @@
       </c>
       <c r="E21" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21" s="33">
         <f t="shared" si="2"/>
@@ -2287,7 +2295,9 @@
       <c r="P21" s="35"/>
       <c r="Q21" s="35"/>
       <c r="R21" s="35"/>
-      <c r="S21" s="35"/>
+      <c r="S21" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="T21" s="35"/>
       <c r="U21" s="35"/>
       <c r="V21" s="35"/>
@@ -2455,7 +2465,7 @@
       </c>
       <c r="E25" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="33">
         <f t="shared" si="2"/>
@@ -2475,7 +2485,9 @@
       <c r="N25" s="35"/>
       <c r="O25" s="35"/>
       <c r="P25" s="35"/>
-      <c r="Q25" s="35"/>
+      <c r="Q25" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="R25" s="35"/>
       <c r="S25" s="35"/>
       <c r="T25" s="35"/>
@@ -2599,7 +2611,7 @@
       </c>
       <c r="E28" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="33">
         <f t="shared" si="2"/>
@@ -2618,7 +2630,9 @@
       <c r="O28" s="35"/>
       <c r="P28" s="35"/>
       <c r="Q28" s="35"/>
-      <c r="R28" s="35"/>
+      <c r="R28" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="S28" s="35"/>
       <c r="T28" s="35"/>
       <c r="U28" s="35"/>
@@ -2645,7 +2659,7 @@
       </c>
       <c r="E29" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F29" s="33">
         <f t="shared" si="2"/>
@@ -2667,7 +2681,9 @@
       <c r="P29" s="35"/>
       <c r="Q29" s="35"/>
       <c r="R29" s="35"/>
-      <c r="S29" s="35"/>
+      <c r="S29" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="T29" s="35"/>
       <c r="U29" s="35"/>
       <c r="V29" s="35"/>
@@ -2795,7 +2811,7 @@
       </c>
       <c r="E32" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F32" s="33">
         <f t="shared" si="2"/>
@@ -2817,7 +2833,9 @@
       <c r="P32" s="35"/>
       <c r="Q32" s="35"/>
       <c r="R32" s="35"/>
-      <c r="S32" s="35"/>
+      <c r="S32" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="T32" s="35"/>
       <c r="U32" s="35"/>
       <c r="V32" s="35"/>
@@ -2843,7 +2861,7 @@
       </c>
       <c r="E33" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F33" s="33">
         <f t="shared" si="2"/>
@@ -2863,7 +2881,9 @@
       <c r="P33" s="35"/>
       <c r="Q33" s="35"/>
       <c r="R33" s="35"/>
-      <c r="S33" s="35"/>
+      <c r="S33" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="T33" s="35"/>
       <c r="U33" s="35"/>
       <c r="V33" s="35"/>
@@ -2991,7 +3011,7 @@
       </c>
       <c r="E36" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F36" s="33">
         <f t="shared" si="2"/>
@@ -3009,8 +3029,12 @@
       <c r="N36" s="35"/>
       <c r="O36" s="35"/>
       <c r="P36" s="35"/>
-      <c r="Q36" s="35"/>
-      <c r="R36" s="35"/>
+      <c r="Q36" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="R36" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="S36" s="35"/>
       <c r="T36" s="35"/>
       <c r="U36" s="35"/>
@@ -3415,7 +3439,7 @@
       </c>
       <c r="E45" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F45" s="33">
         <f t="shared" si="2"/>
@@ -3435,7 +3459,9 @@
       <c r="P45" s="35"/>
       <c r="Q45" s="35"/>
       <c r="R45" s="35"/>
-      <c r="S45" s="35"/>
+      <c r="S45" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="T45" s="35"/>
       <c r="U45" s="35"/>
       <c r="V45" s="35"/>
@@ -3461,7 +3487,7 @@
       </c>
       <c r="E46" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F46" s="33">
         <f t="shared" si="2"/>
@@ -3479,7 +3505,9 @@
       <c r="N46" s="35"/>
       <c r="O46" s="35"/>
       <c r="P46" s="35"/>
-      <c r="Q46" s="35"/>
+      <c r="Q46" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="R46" s="35"/>
       <c r="S46" s="35"/>
       <c r="T46" s="35"/>
@@ -3507,7 +3535,7 @@
       </c>
       <c r="E47" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47" s="33">
         <f t="shared" si="2"/>
@@ -3525,7 +3553,9 @@
       <c r="P47" s="35"/>
       <c r="Q47" s="35"/>
       <c r="R47" s="35"/>
-      <c r="S47" s="35"/>
+      <c r="S47" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="T47" s="35"/>
       <c r="U47" s="35"/>
       <c r="V47" s="35"/>
@@ -3551,7 +3581,7 @@
       </c>
       <c r="E48" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F48" s="33">
         <f t="shared" si="2"/>
@@ -3568,8 +3598,12 @@
       <c r="O48" s="35"/>
       <c r="P48" s="35"/>
       <c r="Q48" s="35"/>
-      <c r="R48" s="35"/>
-      <c r="S48" s="35"/>
+      <c r="R48" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="S48" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="T48" s="35"/>
       <c r="U48" s="35"/>
       <c r="V48" s="35"/>
@@ -3643,7 +3677,7 @@
       </c>
       <c r="E50" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F50" s="33">
         <f t="shared" si="2"/>
@@ -3663,7 +3697,9 @@
       <c r="P50" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="Q50" s="35"/>
+      <c r="Q50" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="R50" s="35"/>
       <c r="S50" s="35"/>
       <c r="T50" s="35"/>
@@ -3691,7 +3727,7 @@
       </c>
       <c r="E51" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F51" s="33">
         <f t="shared" si="2"/>
@@ -3708,7 +3744,9 @@
       <c r="O51" s="35"/>
       <c r="P51" s="35"/>
       <c r="Q51" s="35"/>
-      <c r="R51" s="35"/>
+      <c r="R51" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="S51" s="35"/>
       <c r="T51" s="35"/>
       <c r="U51" s="35"/>
@@ -3827,7 +3865,7 @@
       </c>
       <c r="E54" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F54" s="33">
         <f t="shared" si="2"/>
@@ -3851,7 +3889,9 @@
       </c>
       <c r="Q54" s="35"/>
       <c r="R54" s="35"/>
-      <c r="S54" s="35"/>
+      <c r="S54" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="T54" s="35"/>
       <c r="U54" s="35"/>
       <c r="V54" s="35"/>
@@ -4063,7 +4103,7 @@
       </c>
       <c r="E59" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F59" s="33">
         <f t="shared" si="2"/>
@@ -4079,9 +4119,13 @@
       <c r="N59" s="35"/>
       <c r="O59" s="35"/>
       <c r="P59" s="35"/>
-      <c r="Q59" s="35"/>
+      <c r="Q59" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="R59" s="35"/>
-      <c r="S59" s="35"/>
+      <c r="S59" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="T59" s="35"/>
       <c r="U59" s="35"/>
       <c r="V59" s="35"/>
@@ -4107,7 +4151,7 @@
       </c>
       <c r="E60" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F60" s="33">
         <f t="shared" si="2"/>
@@ -4123,7 +4167,9 @@
       <c r="N60" s="35"/>
       <c r="O60" s="35"/>
       <c r="P60" s="35"/>
-      <c r="Q60" s="35"/>
+      <c r="Q60" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="R60" s="35"/>
       <c r="S60" s="35"/>
       <c r="T60" s="35"/>
@@ -4301,7 +4347,7 @@
       </c>
       <c r="E64" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F64" s="33">
         <f t="shared" si="2"/>
@@ -4321,7 +4367,9 @@
       <c r="P64" s="35"/>
       <c r="Q64" s="35"/>
       <c r="R64" s="35"/>
-      <c r="S64" s="35"/>
+      <c r="S64" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="T64" s="35"/>
       <c r="U64" s="35"/>
       <c r="V64" s="35"/>
@@ -4439,7 +4487,7 @@
       </c>
       <c r="E67" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F67" s="33">
         <f t="shared" si="2"/>
@@ -4461,7 +4509,9 @@
       <c r="P67" s="35"/>
       <c r="Q67" s="35"/>
       <c r="R67" s="35"/>
-      <c r="S67" s="35"/>
+      <c r="S67" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="T67" s="35"/>
       <c r="U67" s="35"/>
       <c r="V67" s="35"/>
@@ -4487,7 +4537,7 @@
       </c>
       <c r="E68" s="26">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F68" s="33">
         <f t="shared" si="2"/>
@@ -4509,9 +4559,15 @@
       <c r="P68" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="Q68" s="35"/>
-      <c r="R68" s="35"/>
-      <c r="S68" s="35"/>
+      <c r="Q68" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="R68" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="S68" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="T68" s="35"/>
       <c r="U68" s="35"/>
       <c r="V68" s="35"/>
@@ -4537,7 +4593,7 @@
       </c>
       <c r="E69" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F69" s="33">
         <f t="shared" si="2"/>
@@ -4556,7 +4612,9 @@
       <c r="O69" s="35"/>
       <c r="P69" s="35"/>
       <c r="Q69" s="35"/>
-      <c r="R69" s="35"/>
+      <c r="R69" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="S69" s="35"/>
       <c r="T69" s="35"/>
       <c r="U69" s="35"/>
@@ -4675,7 +4733,7 @@
       </c>
       <c r="E72" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F72" s="33">
         <f t="shared" si="2"/>
@@ -4697,7 +4755,9 @@
       <c r="P72" s="35"/>
       <c r="Q72" s="35"/>
       <c r="R72" s="35"/>
-      <c r="S72" s="35"/>
+      <c r="S72" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="T72" s="35"/>
       <c r="U72" s="35"/>
       <c r="V72" s="35"/>

</xml_diff>

<commit_message>
Updating attendance files 25th feb
</commit_message>
<xml_diff>
--- a/attendance-files/FA-II/FA-II (A) Attendance Sheet.xlsx
+++ b/attendance-files/FA-II/FA-II (A) Attendance Sheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="171">
   <si>
     <t>Indian Institute of Management Indore</t>
   </si>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="E11" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="33">
         <f t="shared" si="2"/>
@@ -1821,7 +1821,9 @@
       <c r="R11" s="35"/>
       <c r="S11" s="35"/>
       <c r="T11" s="35"/>
-      <c r="U11" s="35"/>
+      <c r="U11" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="V11" s="35"/>
       <c r="W11" s="35"/>
       <c r="X11" s="35"/>
@@ -1899,7 +1901,7 @@
       </c>
       <c r="E13" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" s="33">
         <f t="shared" si="2"/>
@@ -1924,7 +1926,9 @@
       <c r="Q13" s="35"/>
       <c r="R13" s="35"/>
       <c r="S13" s="35"/>
-      <c r="T13" s="35"/>
+      <c r="T13" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="U13" s="35"/>
       <c r="V13" s="35"/>
       <c r="W13" s="35"/>
@@ -1949,7 +1953,7 @@
       </c>
       <c r="E14" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="33">
         <f t="shared" si="2"/>
@@ -1970,7 +1974,9 @@
       <c r="Q14" s="35"/>
       <c r="R14" s="35"/>
       <c r="S14" s="35"/>
-      <c r="T14" s="35"/>
+      <c r="T14" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="U14" s="35"/>
       <c r="V14" s="35"/>
       <c r="W14" s="35"/>
@@ -2043,7 +2049,7 @@
       </c>
       <c r="E16" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="33">
         <f t="shared" si="2"/>
@@ -2063,7 +2069,9 @@
       <c r="R16" s="35"/>
       <c r="S16" s="35"/>
       <c r="T16" s="35"/>
-      <c r="U16" s="35"/>
+      <c r="U16" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="V16" s="35"/>
       <c r="W16" s="35"/>
       <c r="X16" s="35"/>
@@ -2135,7 +2143,7 @@
       </c>
       <c r="E18" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F18" s="33">
         <f t="shared" si="2"/>
@@ -2159,7 +2167,9 @@
       <c r="R18" s="35"/>
       <c r="S18" s="35"/>
       <c r="T18" s="35"/>
-      <c r="U18" s="35"/>
+      <c r="U18" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="V18" s="35"/>
       <c r="W18" s="35"/>
       <c r="X18" s="35"/>
@@ -2227,7 +2237,7 @@
       </c>
       <c r="E20" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="33">
         <f t="shared" si="2"/>
@@ -2246,7 +2256,9 @@
       <c r="Q20" s="35"/>
       <c r="R20" s="35"/>
       <c r="S20" s="35"/>
-      <c r="T20" s="35"/>
+      <c r="T20" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="U20" s="35"/>
       <c r="V20" s="35"/>
       <c r="W20" s="35"/>
@@ -2515,7 +2527,7 @@
       </c>
       <c r="E26" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F26" s="33">
         <f t="shared" si="2"/>
@@ -2538,7 +2550,9 @@
       <c r="Q26" s="35"/>
       <c r="R26" s="35"/>
       <c r="S26" s="35"/>
-      <c r="T26" s="35"/>
+      <c r="T26" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="U26" s="35"/>
       <c r="V26" s="35"/>
       <c r="W26" s="35"/>
@@ -2563,7 +2577,7 @@
       </c>
       <c r="E27" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F27" s="33">
         <f t="shared" si="2"/>
@@ -2587,7 +2601,9 @@
       <c r="R27" s="35"/>
       <c r="S27" s="35"/>
       <c r="T27" s="35"/>
-      <c r="U27" s="35"/>
+      <c r="U27" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="V27" s="35"/>
       <c r="W27" s="35"/>
       <c r="X27" s="35"/>
@@ -2611,7 +2627,7 @@
       </c>
       <c r="E28" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F28" s="33">
         <f t="shared" si="2"/>
@@ -2635,7 +2651,9 @@
       </c>
       <c r="S28" s="35"/>
       <c r="T28" s="35"/>
-      <c r="U28" s="35"/>
+      <c r="U28" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="V28" s="35"/>
       <c r="W28" s="35"/>
       <c r="X28" s="35"/>
@@ -2659,7 +2677,7 @@
       </c>
       <c r="E29" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F29" s="33">
         <f t="shared" si="2"/>
@@ -2684,7 +2702,9 @@
       <c r="S29" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="T29" s="35"/>
+      <c r="T29" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="U29" s="35"/>
       <c r="V29" s="35"/>
       <c r="W29" s="35"/>
@@ -2909,7 +2929,7 @@
       </c>
       <c r="E34" s="26">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F34" s="33">
         <f t="shared" si="2"/>
@@ -2934,7 +2954,9 @@
       <c r="Q34" s="35"/>
       <c r="R34" s="35"/>
       <c r="S34" s="35"/>
-      <c r="T34" s="35"/>
+      <c r="T34" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="U34" s="35"/>
       <c r="V34" s="35"/>
       <c r="W34" s="35"/>
@@ -3207,7 +3229,7 @@
       </c>
       <c r="E40" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F40" s="33">
         <f t="shared" si="2"/>
@@ -3226,8 +3248,10 @@
       <c r="Q40" s="35"/>
       <c r="R40" s="35"/>
       <c r="S40" s="35"/>
-      <c r="T40" s="35"/>
-      <c r="U40" s="35"/>
+      <c r="T40" s="36"/>
+      <c r="U40" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="V40" s="35"/>
       <c r="W40" s="35"/>
       <c r="X40" s="35"/>
@@ -3251,7 +3275,7 @@
       </c>
       <c r="E41" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41" s="33">
         <f t="shared" si="2"/>
@@ -3272,8 +3296,10 @@
       <c r="Q41" s="35"/>
       <c r="R41" s="35"/>
       <c r="S41" s="35"/>
-      <c r="T41" s="35"/>
-      <c r="U41" s="35"/>
+      <c r="T41" s="36"/>
+      <c r="U41" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="V41" s="35"/>
       <c r="W41" s="35"/>
       <c r="X41" s="35"/>
@@ -3387,7 +3413,7 @@
       </c>
       <c r="E44" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F44" s="33">
         <f t="shared" si="2"/>
@@ -3414,8 +3440,10 @@
       <c r="Q44" s="35"/>
       <c r="R44" s="35"/>
       <c r="S44" s="35"/>
-      <c r="T44" s="35"/>
-      <c r="U44" s="35"/>
+      <c r="T44" s="36"/>
+      <c r="U44" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="V44" s="35"/>
       <c r="W44" s="35"/>
       <c r="X44" s="35"/>
@@ -3487,7 +3515,7 @@
       </c>
       <c r="E46" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F46" s="33">
         <f t="shared" si="2"/>
@@ -3510,8 +3538,10 @@
       </c>
       <c r="R46" s="35"/>
       <c r="S46" s="35"/>
-      <c r="T46" s="35"/>
-      <c r="U46" s="35"/>
+      <c r="T46" s="36"/>
+      <c r="U46" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="V46" s="35"/>
       <c r="W46" s="35"/>
       <c r="X46" s="35"/>
@@ -4057,7 +4087,7 @@
       </c>
       <c r="E58" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F58" s="33">
         <f t="shared" si="2"/>
@@ -4079,7 +4109,9 @@
       <c r="R58" s="35"/>
       <c r="S58" s="35"/>
       <c r="T58" s="35"/>
-      <c r="U58" s="35"/>
+      <c r="U58" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="V58" s="35"/>
       <c r="W58" s="35"/>
       <c r="X58" s="35"/>
@@ -4103,7 +4135,7 @@
       </c>
       <c r="E59" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F59" s="33">
         <f t="shared" si="2"/>
@@ -4127,7 +4159,9 @@
         <v>9</v>
       </c>
       <c r="T59" s="35"/>
-      <c r="U59" s="35"/>
+      <c r="U59" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="V59" s="35"/>
       <c r="W59" s="35"/>
       <c r="X59" s="35"/>
@@ -4487,7 +4521,7 @@
       </c>
       <c r="E67" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F67" s="33">
         <f t="shared" si="2"/>
@@ -4512,7 +4546,9 @@
       <c r="S67" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="T67" s="35"/>
+      <c r="T67" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="U67" s="35"/>
       <c r="V67" s="35"/>
       <c r="W67" s="35"/>
@@ -4537,7 +4573,7 @@
       </c>
       <c r="E68" s="26">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F68" s="33">
         <f t="shared" si="2"/>
@@ -4568,8 +4604,12 @@
       <c r="S68" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="T68" s="35"/>
-      <c r="U68" s="35"/>
+      <c r="T68" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="U68" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="V68" s="35"/>
       <c r="W68" s="35"/>
       <c r="X68" s="35"/>
@@ -4687,7 +4727,7 @@
       </c>
       <c r="E71" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F71" s="33">
         <f t="shared" si="2"/>
@@ -4709,7 +4749,9 @@
       <c r="R71" s="35"/>
       <c r="S71" s="35"/>
       <c r="T71" s="35"/>
-      <c r="U71" s="35"/>
+      <c r="U71" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="V71" s="35"/>
       <c r="W71" s="35"/>
       <c r="X71" s="35"/>
@@ -4783,7 +4825,7 @@
       </c>
       <c r="E73" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F73" s="33">
         <f t="shared" si="2"/>
@@ -4804,7 +4846,9 @@
       <c r="Q73" s="35"/>
       <c r="R73" s="35"/>
       <c r="S73" s="35"/>
-      <c r="T73" s="35"/>
+      <c r="T73" s="36" t="s">
+        <v>9</v>
+      </c>
       <c r="U73" s="35"/>
       <c r="V73" s="35"/>
       <c r="W73" s="35"/>

</xml_diff>

<commit_message>
Updating attendance files 7th march
</commit_message>
<xml_diff>
--- a/attendance-files/FA-II/FA-II (A) Attendance Sheet.xlsx
+++ b/attendance-files/FA-II/FA-II (A) Attendance Sheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="171">
   <si>
     <t>Indian Institute of Management Indore</t>
   </si>
@@ -1804,7 +1804,7 @@
       </c>
       <c r="E11" s="26">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F11" s="34">
         <f t="shared" si="2"/>
@@ -1835,7 +1835,9 @@
       <c r="W11" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="X11" s="36"/>
+      <c r="X11" s="37" t="s">
+        <v>9</v>
+      </c>
       <c r="Y11" s="36"/>
       <c r="Z11" s="36"/>
       <c r="AA11" s="36"/>
@@ -1962,7 +1964,7 @@
       </c>
       <c r="E14" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F14" s="34">
         <f t="shared" si="2"/>
@@ -1991,7 +1993,9 @@
         <v>9</v>
       </c>
       <c r="W14" s="36"/>
-      <c r="X14" s="36"/>
+      <c r="X14" s="37" t="s">
+        <v>9</v>
+      </c>
       <c r="Y14" s="36"/>
       <c r="Z14" s="36"/>
       <c r="AA14" s="36"/>
@@ -2356,7 +2360,7 @@
       </c>
       <c r="E22" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F22" s="34">
         <f t="shared" si="2"/>
@@ -2381,7 +2385,9 @@
         <v>9</v>
       </c>
       <c r="W22" s="36"/>
-      <c r="X22" s="36"/>
+      <c r="X22" s="37" t="s">
+        <v>9</v>
+      </c>
       <c r="Y22" s="36"/>
       <c r="Z22" s="36"/>
       <c r="AA22" s="36"/>
@@ -2450,7 +2456,7 @@
       </c>
       <c r="E24" s="26">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F24" s="34">
         <f t="shared" si="2"/>
@@ -2483,7 +2489,9 @@
       <c r="W24" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="X24" s="36"/>
+      <c r="X24" s="37" t="s">
+        <v>9</v>
+      </c>
       <c r="Y24" s="36"/>
       <c r="Z24" s="36"/>
       <c r="AA24" s="36"/>
@@ -2554,7 +2562,7 @@
       </c>
       <c r="E26" s="26">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F26" s="34">
         <f t="shared" si="2"/>
@@ -2585,7 +2593,9 @@
       <c r="W26" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="X26" s="36"/>
+      <c r="X26" s="37" t="s">
+        <v>9</v>
+      </c>
       <c r="Y26" s="36"/>
       <c r="Z26" s="36"/>
       <c r="AA26" s="36"/>
@@ -2658,7 +2668,7 @@
       </c>
       <c r="E28" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F28" s="34">
         <f t="shared" si="2"/>
@@ -2687,7 +2697,9 @@
       </c>
       <c r="V28" s="36"/>
       <c r="W28" s="36"/>
-      <c r="X28" s="36"/>
+      <c r="X28" s="37" t="s">
+        <v>9</v>
+      </c>
       <c r="Y28" s="36"/>
       <c r="Z28" s="36"/>
       <c r="AA28" s="36"/>
@@ -2862,7 +2874,7 @@
       </c>
       <c r="E32" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F32" s="34">
         <f t="shared" si="2"/>
@@ -2891,7 +2903,9 @@
       <c r="U32" s="36"/>
       <c r="V32" s="36"/>
       <c r="W32" s="36"/>
-      <c r="X32" s="36"/>
+      <c r="X32" s="37" t="s">
+        <v>9</v>
+      </c>
       <c r="Y32" s="36"/>
       <c r="Z32" s="36"/>
       <c r="AA32" s="36"/>
@@ -3166,7 +3180,7 @@
       </c>
       <c r="E38" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F38" s="34">
         <f t="shared" si="2"/>
@@ -3195,7 +3209,9 @@
         <v>9</v>
       </c>
       <c r="W38" s="36"/>
-      <c r="X38" s="36"/>
+      <c r="X38" s="37" t="s">
+        <v>9</v>
+      </c>
       <c r="Y38" s="36"/>
       <c r="Z38" s="36"/>
       <c r="AA38" s="36"/>
@@ -3802,7 +3818,7 @@
       </c>
       <c r="E51" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F51" s="34">
         <f t="shared" si="2"/>
@@ -3827,7 +3843,9 @@
       <c r="U51" s="36"/>
       <c r="V51" s="36"/>
       <c r="W51" s="36"/>
-      <c r="X51" s="36"/>
+      <c r="X51" s="37" t="s">
+        <v>9</v>
+      </c>
       <c r="Y51" s="36"/>
       <c r="Z51" s="36"/>
       <c r="AA51" s="36"/>
@@ -4088,7 +4106,7 @@
       </c>
       <c r="E57" s="26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F57" s="34">
         <f t="shared" si="2"/>
@@ -4115,7 +4133,9 @@
         <v>9</v>
       </c>
       <c r="W57" s="36"/>
-      <c r="X57" s="36"/>
+      <c r="X57" s="37" t="s">
+        <v>9</v>
+      </c>
       <c r="Y57" s="36"/>
       <c r="Z57" s="36"/>
       <c r="AA57" s="36"/>
@@ -4184,7 +4204,7 @@
       </c>
       <c r="E59" s="26">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F59" s="34">
         <f t="shared" si="2"/>
@@ -4213,7 +4233,9 @@
       </c>
       <c r="V59" s="36"/>
       <c r="W59" s="36"/>
-      <c r="X59" s="36"/>
+      <c r="X59" s="37" t="s">
+        <v>9</v>
+      </c>
       <c r="Y59" s="36"/>
       <c r="Z59" s="36"/>
       <c r="AA59" s="36"/>
@@ -4530,7 +4552,7 @@
       </c>
       <c r="E66" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F66" s="34">
         <f t="shared" si="2"/>
@@ -4557,7 +4579,9 @@
         <v>9</v>
       </c>
       <c r="W66" s="36"/>
-      <c r="X66" s="36"/>
+      <c r="X66" s="37" t="s">
+        <v>9</v>
+      </c>
       <c r="Y66" s="36"/>
       <c r="Z66" s="36"/>
       <c r="AA66" s="36"/>
@@ -4630,7 +4654,7 @@
       </c>
       <c r="E68" s="26">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F68" s="34">
         <f t="shared" si="2"/>
@@ -4673,7 +4697,9 @@
       <c r="W68" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="X68" s="36"/>
+      <c r="X68" s="37" t="s">
+        <v>9</v>
+      </c>
       <c r="Y68" s="36"/>
       <c r="Z68" s="36"/>
       <c r="AA68" s="36"/>
@@ -4694,7 +4720,7 @@
       </c>
       <c r="E69" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F69" s="34">
         <f t="shared" si="2"/>
@@ -4721,7 +4747,9 @@
       <c r="U69" s="36"/>
       <c r="V69" s="36"/>
       <c r="W69" s="36"/>
-      <c r="X69" s="36"/>
+      <c r="X69" s="37" t="s">
+        <v>9</v>
+      </c>
       <c r="Y69" s="36"/>
       <c r="Z69" s="36"/>
       <c r="AA69" s="36"/>
@@ -5040,7 +5068,7 @@
       </c>
       <c r="E76" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F76" s="34">
         <f t="shared" si="2"/>
@@ -5069,7 +5097,9 @@
         <v>9</v>
       </c>
       <c r="W76" s="36"/>
-      <c r="X76" s="36"/>
+      <c r="X76" s="37" t="s">
+        <v>9</v>
+      </c>
       <c r="Y76" s="36"/>
       <c r="Z76" s="36"/>
       <c r="AA76" s="36"/>
@@ -5136,7 +5166,7 @@
       </c>
       <c r="E78" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F78" s="34">
         <f t="shared" si="2"/>
@@ -5163,7 +5193,9 @@
       <c r="W78" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="X78" s="36"/>
+      <c r="X78" s="37" t="s">
+        <v>9</v>
+      </c>
       <c r="Y78" s="36"/>
       <c r="Z78" s="36"/>
       <c r="AA78" s="36"/>

</xml_diff>

<commit_message>
updated files on 12 march
</commit_message>
<xml_diff>
--- a/attendance-files/FA-II/FA-II (A) Attendance Sheet.xlsx
+++ b/attendance-files/FA-II/FA-II (A) Attendance Sheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="171">
   <si>
     <t>Indian Institute of Management Indore</t>
   </si>
@@ -1664,7 +1664,7 @@
       </c>
       <c r="E8" s="26">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" s="34">
         <f t="shared" si="2"/>
@@ -1692,9 +1692,7 @@
       <c r="V8" s="36"/>
       <c r="W8" s="36"/>
       <c r="X8" s="36"/>
-      <c r="Y8" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="Y8" s="36"/>
       <c r="Z8" s="36"/>
       <c r="AA8" s="36"/>
     </row>
@@ -1714,7 +1712,7 @@
       </c>
       <c r="E9" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" s="34">
         <f t="shared" si="2"/>
@@ -1742,9 +1740,7 @@
       <c r="V9" s="36"/>
       <c r="W9" s="36"/>
       <c r="X9" s="36"/>
-      <c r="Y9" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="Y9" s="36"/>
       <c r="Z9" s="36"/>
       <c r="AA9" s="36"/>
     </row>
@@ -2412,7 +2408,7 @@
       </c>
       <c r="E23" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" s="34">
         <f t="shared" si="2"/>
@@ -2440,9 +2436,7 @@
         <v>9</v>
       </c>
       <c r="X23" s="36"/>
-      <c r="Y23" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="Y23" s="36"/>
       <c r="Z23" s="36"/>
       <c r="AA23" s="36"/>
     </row>
@@ -2462,7 +2456,7 @@
       </c>
       <c r="E24" s="26">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F24" s="34">
         <f t="shared" si="2"/>
@@ -2498,9 +2492,7 @@
       <c r="X24" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="Y24" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="Y24" s="36"/>
       <c r="Z24" s="36"/>
       <c r="AA24" s="36"/>
     </row>
@@ -2570,7 +2562,7 @@
       </c>
       <c r="E26" s="26">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F26" s="34">
         <f t="shared" si="2"/>
@@ -2604,9 +2596,7 @@
       <c r="X26" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="Y26" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="Y26" s="36"/>
       <c r="Z26" s="36"/>
       <c r="AA26" s="36"/>
     </row>
@@ -2678,7 +2668,7 @@
       </c>
       <c r="E28" s="26">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" s="34">
         <f t="shared" si="2"/>
@@ -2710,9 +2700,7 @@
       <c r="X28" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="Y28" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="Y28" s="36"/>
       <c r="Z28" s="36"/>
       <c r="AA28" s="36"/>
     </row>
@@ -2886,7 +2874,7 @@
       </c>
       <c r="E32" s="26">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32" s="34">
         <f t="shared" si="2"/>
@@ -2918,9 +2906,7 @@
       <c r="X32" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="Y32" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="Y32" s="36"/>
       <c r="Z32" s="36"/>
       <c r="AA32" s="36"/>
     </row>
@@ -2940,7 +2926,7 @@
       </c>
       <c r="E33" s="26">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33" s="34">
         <f t="shared" si="2"/>
@@ -2968,9 +2954,7 @@
       <c r="V33" s="36"/>
       <c r="W33" s="36"/>
       <c r="X33" s="36"/>
-      <c r="Y33" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="Y33" s="36"/>
       <c r="Z33" s="36"/>
       <c r="AA33" s="36"/>
     </row>
@@ -3094,7 +3078,7 @@
       </c>
       <c r="E36" s="26">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F36" s="34">
         <f t="shared" si="2"/>
@@ -3124,9 +3108,7 @@
       <c r="V36" s="36"/>
       <c r="W36" s="36"/>
       <c r="X36" s="36"/>
-      <c r="Y36" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="Y36" s="36"/>
       <c r="Z36" s="36"/>
       <c r="AA36" s="36"/>
     </row>
@@ -3296,7 +3278,7 @@
       </c>
       <c r="E40" s="26">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" s="34">
         <f t="shared" si="2"/>
@@ -3324,9 +3306,7 @@
       </c>
       <c r="W40" s="36"/>
       <c r="X40" s="36"/>
-      <c r="Y40" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="Y40" s="36"/>
       <c r="Z40" s="36"/>
       <c r="AA40" s="36"/>
     </row>
@@ -3346,7 +3326,7 @@
       </c>
       <c r="E41" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" s="34">
         <f t="shared" si="2"/>
@@ -3374,9 +3354,7 @@
       <c r="V41" s="36"/>
       <c r="W41" s="36"/>
       <c r="X41" s="36"/>
-      <c r="Y41" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="Y41" s="36"/>
       <c r="Z41" s="36"/>
       <c r="AA41" s="36"/>
     </row>
@@ -3396,7 +3374,7 @@
       </c>
       <c r="E42" s="26">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" s="34">
         <f t="shared" si="2"/>
@@ -3424,9 +3402,7 @@
       </c>
       <c r="W42" s="36"/>
       <c r="X42" s="36"/>
-      <c r="Y42" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="Y42" s="36"/>
       <c r="Z42" s="36"/>
       <c r="AA42" s="36"/>
     </row>
@@ -3646,7 +3622,7 @@
       </c>
       <c r="E47" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" s="34">
         <f t="shared" si="2"/>
@@ -3672,9 +3648,7 @@
       <c r="V47" s="36"/>
       <c r="W47" s="36"/>
       <c r="X47" s="36"/>
-      <c r="Y47" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="Y47" s="36"/>
       <c r="Z47" s="36"/>
       <c r="AA47" s="36"/>
     </row>
@@ -3744,7 +3718,7 @@
       </c>
       <c r="E49" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" s="34">
         <f t="shared" si="2"/>
@@ -3772,9 +3746,7 @@
       <c r="V49" s="36"/>
       <c r="W49" s="36"/>
       <c r="X49" s="36"/>
-      <c r="Y49" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="Y49" s="36"/>
       <c r="Z49" s="36"/>
       <c r="AA49" s="36"/>
     </row>
@@ -3794,7 +3766,7 @@
       </c>
       <c r="E50" s="26">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F50" s="34">
         <f t="shared" si="2"/>
@@ -3826,9 +3798,7 @@
         <v>9</v>
       </c>
       <c r="X50" s="36"/>
-      <c r="Y50" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="Y50" s="36"/>
       <c r="Z50" s="36"/>
       <c r="AA50" s="36"/>
     </row>
@@ -3848,7 +3818,7 @@
       </c>
       <c r="E51" s="26">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" s="34">
         <f t="shared" si="2"/>
@@ -3876,9 +3846,7 @@
       <c r="X51" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="Y51" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="Y51" s="36"/>
       <c r="Z51" s="36"/>
       <c r="AA51" s="36"/>
     </row>
@@ -4138,7 +4106,7 @@
       </c>
       <c r="E57" s="26">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" s="34">
         <f t="shared" si="2"/>
@@ -4168,9 +4136,7 @@
       <c r="X57" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="Y57" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="Y57" s="36"/>
       <c r="Z57" s="36"/>
       <c r="AA57" s="36"/>
     </row>
@@ -4390,7 +4356,7 @@
       </c>
       <c r="E62" s="26">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F62" s="34">
         <f t="shared" si="2"/>
@@ -4420,9 +4386,7 @@
         <v>9</v>
       </c>
       <c r="X62" s="36"/>
-      <c r="Y62" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="Y62" s="36"/>
       <c r="Z62" s="36"/>
       <c r="AA62" s="36"/>
     </row>
@@ -4492,7 +4456,7 @@
       </c>
       <c r="E64" s="26">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" s="34">
         <f t="shared" si="2"/>
@@ -4520,9 +4484,7 @@
       <c r="V64" s="36"/>
       <c r="W64" s="36"/>
       <c r="X64" s="36"/>
-      <c r="Y64" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="Y64" s="36"/>
       <c r="Z64" s="36"/>
       <c r="AA64" s="36"/>
     </row>
@@ -4692,7 +4654,7 @@
       </c>
       <c r="E68" s="26">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F68" s="34">
         <f t="shared" si="2"/>
@@ -4738,9 +4700,7 @@
       <c r="X68" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="Y68" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="Y68" s="36"/>
       <c r="Z68" s="36"/>
       <c r="AA68" s="36"/>
     </row>
@@ -4856,7 +4816,7 @@
       </c>
       <c r="E71" s="26">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F71" s="34">
         <f t="shared" si="2"/>
@@ -4886,9 +4846,7 @@
       </c>
       <c r="W71" s="36"/>
       <c r="X71" s="36"/>
-      <c r="Y71" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="Y71" s="36"/>
       <c r="Z71" s="36"/>
       <c r="AA71" s="36"/>
     </row>
@@ -5258,7 +5216,7 @@
       </c>
       <c r="E79" s="26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F79" s="34">
         <f t="shared" si="2"/>
@@ -5284,9 +5242,7 @@
       <c r="V79" s="36"/>
       <c r="W79" s="36"/>
       <c r="X79" s="36"/>
-      <c r="Y79" s="37" t="s">
-        <v>9</v>
-      </c>
+      <c r="Y79" s="36"/>
       <c r="Z79" s="36"/>
       <c r="AA79" s="36"/>
     </row>

</xml_diff>